<commit_message>
Complete data proposal section
</commit_message>
<xml_diff>
--- a/data/table_Transportation.xlsx
+++ b/data/table_Transportation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\EIA-861\Publications\Results\ESR\2022\XML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramadityailham/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5D4E57A-B1AD-4829-A2C7-7FD1B8713716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CB0AE5-51E1-D54A-9A8A-02CEBD365E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 9" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table 9'!$A$3:$G$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table 9'!$A$1:$G$44</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Table 9'!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
-  <si>
-    <t>2022 Utility Bundled Retail Sales- Transportation</t>
-  </si>
-  <si>
-    <t>(Data from forms EIA-861- schedules 4A &amp; 4D and EIA-861S)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
   <si>
     <t>Entity</t>
   </si>
@@ -272,9 +266,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -830,7 +824,7 @@
     <xf numFmtId="3" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1190,411 +1184,447 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="42.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>213</v>
+      </c>
+      <c r="F2" s="7">
+        <v>33</v>
+      </c>
+      <c r="G2" s="8">
+        <v>15.492958</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>6</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="G3" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>9375</v>
+      </c>
+      <c r="F4" s="7">
+        <v>866</v>
+      </c>
+      <c r="G4" s="8">
+        <v>9.2373332999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>829</v>
+      </c>
+      <c r="F5" s="7">
+        <v>115.5</v>
+      </c>
+      <c r="G5" s="8">
+        <v>13.932449</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6">
-        <v>213</v>
-      </c>
-      <c r="F4" s="7">
-        <v>33</v>
-      </c>
-      <c r="G4" s="8">
-        <v>15.492958</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6">
-        <v>6</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="G5" s="8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D6" s="6">
         <v>1</v>
       </c>
       <c r="E6" s="6">
-        <v>9375</v>
+        <v>93808</v>
       </c>
       <c r="F6" s="7">
-        <v>866</v>
+        <v>12338.1</v>
       </c>
       <c r="G6" s="8">
-        <v>9.2373332999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13.152502999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
       </c>
       <c r="E7" s="6">
-        <v>829</v>
+        <v>6968</v>
       </c>
       <c r="F7" s="7">
-        <v>115.5</v>
+        <v>1322.7</v>
       </c>
       <c r="G7" s="8">
-        <v>13.932449</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18.982491</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="E8" s="6">
-        <v>93808</v>
+        <v>909</v>
       </c>
       <c r="F8" s="7">
-        <v>12338.1</v>
+        <v>172.7</v>
       </c>
       <c r="G8" s="8">
-        <v>13.152502999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18.998899999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="6">
-        <v>6968</v>
+        <v>105994</v>
       </c>
       <c r="F9" s="7">
-        <v>1322.7</v>
+        <v>21078.2</v>
       </c>
       <c r="G9" s="8">
-        <v>18.982491</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19.886220000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
       </c>
       <c r="E10" s="6">
-        <v>909</v>
+        <v>26447</v>
       </c>
       <c r="F10" s="7">
-        <v>172.7</v>
+        <v>3889.3</v>
       </c>
       <c r="G10" s="8">
-        <v>18.998899999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14.706016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" s="6">
-        <v>105994</v>
+        <v>79128</v>
       </c>
       <c r="F11" s="7">
-        <v>21078.2</v>
+        <v>14284.5</v>
       </c>
       <c r="G11" s="8">
-        <v>19.886220000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18.052396000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
       </c>
       <c r="E12" s="6">
-        <v>26447</v>
+        <v>3691</v>
       </c>
       <c r="F12" s="7">
-        <v>3889.3</v>
+        <v>300.8</v>
       </c>
       <c r="G12" s="8">
-        <v>14.706016</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.1495529999999992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D13" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E13" s="6">
-        <v>79128</v>
+        <v>91360</v>
       </c>
       <c r="F13" s="7">
-        <v>14284.5</v>
+        <v>9056.7999999999993</v>
       </c>
       <c r="G13" s="8">
-        <v>18.052396000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.9133099999999992</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D14" s="6">
         <v>1</v>
       </c>
       <c r="E14" s="6">
-        <v>3691</v>
+        <v>122654</v>
       </c>
       <c r="F14" s="7">
-        <v>300.8</v>
+        <v>23646.7</v>
       </c>
       <c r="G14" s="8">
-        <v>8.1495529999999992</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19.279191999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
       </c>
       <c r="E15" s="6">
-        <v>91360</v>
+        <v>11291</v>
       </c>
       <c r="F15" s="7">
-        <v>9056.7999999999993</v>
+        <v>2251.6999999999998</v>
       </c>
       <c r="G15" s="8">
-        <v>9.9133099999999992</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19.942432</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D16" s="6">
         <v>1</v>
       </c>
       <c r="E16" s="6">
-        <v>122654</v>
+        <v>71178</v>
       </c>
       <c r="F16" s="7">
-        <v>23646.7</v>
+        <v>7238.7</v>
       </c>
       <c r="G16" s="8">
-        <v>19.279191999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.169855999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
       </c>
       <c r="E17" s="6">
-        <v>11291</v>
+        <v>3921</v>
       </c>
       <c r="F17" s="7">
-        <v>2251.6999999999998</v>
+        <v>415.9</v>
       </c>
       <c r="G17" s="8">
-        <v>19.942432</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.606987999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
       </c>
       <c r="E18" s="6">
-        <v>71178</v>
+        <v>143691</v>
       </c>
       <c r="F18" s="7">
-        <v>7238.7</v>
+        <v>13400.2</v>
       </c>
       <c r="G18" s="8">
-        <v>10.169855999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.3257059000000009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>11</v>
@@ -1603,638 +1633,592 @@
         <v>1</v>
       </c>
       <c r="E19" s="6">
-        <v>3921</v>
+        <v>18518</v>
       </c>
       <c r="F19" s="7">
-        <v>415.9</v>
+        <v>1458.7</v>
       </c>
       <c r="G19" s="8">
-        <v>10.606987999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7.8772006000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
       </c>
       <c r="E20" s="6">
-        <v>143691</v>
+        <v>12518</v>
       </c>
       <c r="F20" s="7">
-        <v>13400.2</v>
+        <v>1631</v>
       </c>
       <c r="G20" s="8">
-        <v>9.3257059000000009</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13.029237999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
       </c>
       <c r="E21" s="6">
-        <v>18518</v>
+        <v>10181</v>
       </c>
       <c r="F21" s="7">
-        <v>1458.7</v>
+        <v>1267.0999999999999</v>
       </c>
       <c r="G21" s="8">
-        <v>7.8772006000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12.445732</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D22" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" s="6">
-        <v>12518</v>
+        <v>4320</v>
       </c>
       <c r="F22" s="7">
-        <v>1631</v>
+        <v>533.70000000000005</v>
       </c>
       <c r="G22" s="8">
-        <v>13.029237999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12.354167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
       </c>
       <c r="E23" s="6">
-        <v>10181</v>
+        <v>19941</v>
       </c>
       <c r="F23" s="7">
-        <v>1267.0999999999999</v>
+        <v>2450.1999999999998</v>
       </c>
       <c r="G23" s="8">
-        <v>12.445732</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12.287247000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D24" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="6">
-        <v>4320</v>
+        <v>1875</v>
       </c>
       <c r="F24" s="7">
-        <v>533.70000000000005</v>
+        <v>214.7</v>
       </c>
       <c r="G24" s="8">
-        <v>12.354167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.450666999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D25" s="6">
         <v>1</v>
       </c>
       <c r="E25" s="6">
-        <v>19941</v>
+        <v>23233</v>
       </c>
       <c r="F25" s="7">
-        <v>2450.1999999999998</v>
+        <v>2037.2</v>
       </c>
       <c r="G25" s="8">
-        <v>12.287247000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.7685619999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D26" s="6">
         <v>1</v>
       </c>
       <c r="E26" s="6">
-        <v>1875</v>
+        <v>14681</v>
       </c>
       <c r="F26" s="7">
-        <v>214.7</v>
+        <v>1117.2</v>
       </c>
       <c r="G26" s="8">
-        <v>11.450666999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7.6098357999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27" s="6">
-        <v>23233</v>
+        <v>3450</v>
       </c>
       <c r="F27" s="7">
-        <v>2037.2</v>
+        <v>870.4</v>
       </c>
       <c r="G27" s="8">
-        <v>8.7685619999999993</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25.228985999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D28" s="6">
         <v>1</v>
       </c>
       <c r="E28" s="6">
-        <v>14681</v>
+        <v>7176</v>
       </c>
       <c r="F28" s="7">
-        <v>1117.2</v>
+        <v>698.6</v>
       </c>
       <c r="G28" s="8">
-        <v>7.6098357999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.7352284999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D29" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="6">
-        <v>3450</v>
+        <v>10608</v>
       </c>
       <c r="F29" s="7">
-        <v>870.4</v>
+        <v>2237</v>
       </c>
       <c r="G29" s="8">
-        <v>25.228985999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21.087858000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D30" s="6">
         <v>1</v>
       </c>
       <c r="E30" s="6">
-        <v>7176</v>
+        <v>273792</v>
       </c>
       <c r="F30" s="7">
-        <v>698.6</v>
+        <v>46015.6</v>
       </c>
       <c r="G30" s="8">
-        <v>9.7352284999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16.806773</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D31" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="6">
-        <v>10608</v>
+        <v>16083</v>
       </c>
       <c r="F31" s="7">
-        <v>2237</v>
+        <v>2096.5</v>
       </c>
       <c r="G31" s="8">
-        <v>21.087858000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13.035503</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D32" s="6">
         <v>1</v>
       </c>
       <c r="E32" s="6">
-        <v>273792</v>
+        <v>2805</v>
       </c>
       <c r="F32" s="7">
-        <v>46015.6</v>
+        <v>275</v>
       </c>
       <c r="G32" s="8">
-        <v>16.806773</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.8039216000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D33" s="6">
         <v>1</v>
       </c>
       <c r="E33" s="6">
-        <v>16083</v>
+        <v>14346</v>
       </c>
       <c r="F33" s="7">
-        <v>2096.5</v>
+        <v>1538.1</v>
       </c>
       <c r="G33" s="8">
-        <v>13.035503</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.721455000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D34" s="6">
         <v>1</v>
       </c>
       <c r="E34" s="6">
-        <v>2805</v>
+        <v>8353</v>
       </c>
       <c r="F34" s="7">
-        <v>275</v>
+        <v>834</v>
       </c>
       <c r="G34" s="8">
-        <v>9.8039216000000007</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.9844366999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D35" s="6">
         <v>1</v>
       </c>
       <c r="E35" s="6">
-        <v>14346</v>
+        <v>992</v>
       </c>
       <c r="F35" s="7">
-        <v>1538.1</v>
+        <v>88</v>
       </c>
       <c r="G35" s="8">
-        <v>10.721455000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.8709676999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D36" s="6">
         <v>1</v>
       </c>
       <c r="E36" s="6">
-        <v>8353</v>
+        <v>6074</v>
       </c>
       <c r="F36" s="7">
-        <v>834</v>
+        <v>709.7</v>
       </c>
       <c r="G36" s="8">
-        <v>9.9844366999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.684227999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="D37" s="6">
         <v>1</v>
       </c>
       <c r="E37" s="6">
-        <v>992</v>
+        <v>11481</v>
       </c>
       <c r="F37" s="7">
-        <v>88</v>
+        <v>420.6</v>
       </c>
       <c r="G37" s="8">
-        <v>8.8709676999999996</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.6634440000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="C38" s="5" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="D38" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="6">
-        <v>6074</v>
+        <v>168171</v>
       </c>
       <c r="F38" s="7">
-        <v>709.7</v>
+        <v>11838</v>
       </c>
       <c r="G38" s="8">
-        <v>11.684227999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7.0392636</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="D39" s="6">
         <v>1</v>
       </c>
       <c r="E39" s="6">
-        <v>11481</v>
+        <v>46004</v>
       </c>
       <c r="F39" s="7">
-        <v>420.6</v>
+        <v>5693.7</v>
       </c>
       <c r="G39" s="8">
-        <v>3.6634440000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12.376531999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="D40" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40" s="6">
-        <v>168171</v>
+        <v>129802</v>
       </c>
       <c r="F40" s="7">
-        <v>11838</v>
+        <v>14086.9</v>
       </c>
       <c r="G40" s="8">
-        <v>7.0392636</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.852606</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D41" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E41" s="6">
-        <v>46004</v>
+        <v>108029</v>
       </c>
       <c r="F41" s="7">
-        <v>5693.7</v>
+        <v>10789.4</v>
       </c>
       <c r="G41" s="8">
-        <v>12.376531999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.9875033999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D42" s="6">
         <v>1</v>
       </c>
       <c r="E42" s="6">
-        <v>129802</v>
+        <v>767</v>
       </c>
       <c r="F42" s="7">
-        <v>14086.9</v>
+        <v>66.7</v>
       </c>
       <c r="G42" s="8">
-        <v>10.852606</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.6962189999999993</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E43" s="6">
-        <v>108029</v>
+        <v>5137</v>
       </c>
       <c r="F43" s="7">
-        <v>10789.4</v>
+        <v>591.20000000000005</v>
       </c>
       <c r="G43" s="8">
-        <v>9.9875033999999996</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.508663</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="6">
-        <v>767</v>
+        <v>1101</v>
       </c>
       <c r="F44" s="7">
-        <v>66.7</v>
+        <v>182.2</v>
       </c>
       <c r="G44" s="8">
-        <v>8.6962189999999993</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="6">
-        <v>1</v>
-      </c>
-      <c r="E45" s="6">
-        <v>5137</v>
-      </c>
-      <c r="F45" s="7">
-        <v>591.20000000000005</v>
-      </c>
-      <c r="G45" s="8">
-        <v>11.508663</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="6">
-        <v>2</v>
-      </c>
-      <c r="E46" s="6">
-        <v>1101</v>
-      </c>
-      <c r="F46" s="7">
-        <v>182.2</v>
-      </c>
-      <c r="G46" s="8">
         <v>16.548591999999999</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G46"/>
+  <autoFilter ref="A1:G44" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="1000" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>